<commit_message>
feat: add supplier page
</commit_message>
<xml_diff>
--- a/public/example-warehouses-import.xlsx
+++ b/public/example-warehouses-import.xlsx
@@ -1,113 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\semen\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{38CA5D73-C998-47DA-AE66-0C41CF3EBBF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>country</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>phone</t>
-  </si>
-  <si>
-    <t>contactPerson</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>zipCode</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>imageUrl</t>
-  </si>
-  <si>
-    <t>Jessamine Melendez</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eiusmod id expedita </t>
-  </si>
-  <si>
-    <t>In aliqua Consequun</t>
-  </si>
-  <si>
-    <t>+1 (347) 385-4869</t>
-  </si>
-  <si>
-    <t>Nesciunt quam qui e</t>
-  </si>
-  <si>
-    <t>gijoduqebe@mailinator.com</t>
-  </si>
-  <si>
-    <t>50155</t>
-  </si>
-  <si>
-    <t>DISABLED</t>
-  </si>
-  <si>
-    <t>https://utfs.io/f/077ddb63-e310-4a9f-92ba-2f58fa861c50-e3beai.png</t>
-  </si>
-  <si>
-    <t>Zahir Munoz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consectetur et quia </t>
-  </si>
-  <si>
-    <t>Amet itaque officia</t>
-  </si>
-  <si>
-    <t>+1 (384) 326-7541</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quo consequatur est </t>
-  </si>
-  <si>
-    <t>mysajino@mailinator.com</t>
-  </si>
-  <si>
-    <t>12613</t>
-  </si>
-  <si>
-    <t>ACTIVE</t>
-  </si>
-  <si>
-    <t>/placeholder.svg</t>
-  </si>
-</sst>
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -137,21 +65,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -476,103 +396,191 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:I3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>id</v>
+      </c>
+      <c r="B1" t="str">
+        <v>name</v>
+      </c>
+      <c r="C1" t="str">
+        <v>slug</v>
+      </c>
+      <c r="D1" t="str">
+        <v>country</v>
+      </c>
+      <c r="E1" t="str">
+        <v>state</v>
+      </c>
+      <c r="F1" t="str">
+        <v>city</v>
+      </c>
+      <c r="G1" t="str">
+        <v>phone</v>
+      </c>
+      <c r="H1" t="str">
+        <v>contactPerson</v>
+      </c>
+      <c r="I1" t="str">
+        <v>email</v>
+      </c>
+      <c r="J1" t="str">
+        <v>zipCode</v>
+      </c>
+      <c r="K1" t="str">
+        <v>status</v>
+      </c>
+      <c r="L1" t="str">
+        <v>imageUrl</v>
+      </c>
+      <c r="M1" t="str">
+        <v>createdAt</v>
+      </c>
+      <c r="N1" t="str">
+        <v>updatedAt</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>6669c7ac01ebe2e0fda50ec1</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Not not</v>
+      </c>
+      <c r="C2" t="str">
+        <v>not-not</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Australia</v>
+      </c>
+      <c r="E2" t="str">
+        <v>Tasmania</v>
+      </c>
+      <c r="F2" t="str">
+        <v>Blackstone Heights</v>
+      </c>
+      <c r="G2" t="str">
+        <v>09182738</v>
+      </c>
+      <c r="H2" t="str">
+        <v>Manuka</v>
+      </c>
+      <c r="I2" t="str">
+        <v>tuyul9923@gmail.com</v>
+      </c>
+      <c r="J2" t="str">
+        <v>373737</v>
+      </c>
+      <c r="K2" t="str">
+        <v>ACTIVE</v>
+      </c>
+      <c r="L2" t="str">
+        <v>/placeholder.svg</v>
+      </c>
+      <c r="M2" t="str">
+        <v>2024-06-12T16:07:08.532Z</v>
+      </c>
+      <c r="N2" t="str">
+        <v>2024-06-12T16:07:08.532Z</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" t="s">
-        <v>26</v>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>666963cc890bc8d0462f6015</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Silas Hopper</v>
+      </c>
+      <c r="C3" t="str">
+        <v>silas-hopper</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Indonesia</v>
+      </c>
+      <c r="E3" t="str">
+        <v>Sumatera Barat</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Kabupaten Pasaman Barat</v>
+      </c>
+      <c r="G3" t="str">
+        <v>+1 (662) 948-9162</v>
+      </c>
+      <c r="H3" t="str">
+        <v>Velit amet nemo mai</v>
+      </c>
+      <c r="I3" t="str">
+        <v>bozemosar@mailinator.com</v>
+      </c>
+      <c r="J3" t="str">
+        <v>54837</v>
+      </c>
+      <c r="K3" t="str">
+        <v>DISABLED</v>
+      </c>
+      <c r="L3" t="str">
+        <v>/placeholder.svg</v>
+      </c>
+      <c r="M3" t="str">
+        <v>2024-06-12T09:01:00.360Z</v>
+      </c>
+      <c r="N3" t="str">
+        <v>2024-06-12T09:01:00.360Z</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>6669611243e52b6563e95edc</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Hedwig Camacho</v>
+      </c>
+      <c r="C4" t="str">
+        <v>hedwig-camacho</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Indonesia</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Gorontalo</v>
+      </c>
+      <c r="F4" t="str">
+        <v>Kabupaten Boalemo</v>
+      </c>
+      <c r="G4" t="str">
+        <v>+1 (578) 255-1126</v>
+      </c>
+      <c r="H4" t="str">
+        <v>Et dignissimos labor</v>
+      </c>
+      <c r="I4" t="str">
+        <v>duxosoce@mailinator.com</v>
+      </c>
+      <c r="J4" t="str">
+        <v>28196</v>
+      </c>
+      <c r="K4" t="str">
+        <v>ACTIVE</v>
+      </c>
+      <c r="L4" t="str">
+        <v>/placeholder.svg</v>
+      </c>
+      <c r="M4" t="str">
+        <v>2024-06-12T08:49:22.987Z</v>
+      </c>
+      <c r="N4" t="str">
+        <v>2024-06-12T09:00:25.834Z</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:N4"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>